<commit_message>
add student_id and staff_id
</commit_message>
<xml_diff>
--- a/main/static/records/Grade1.xlsx
+++ b/main/static/records/Grade1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="253">
   <si>
     <t xml:space="preserve">RFID NUMBER</t>
   </si>
@@ -43,6 +43,12 @@
     <t xml:space="preserve">EMERGENCY CONTACT NUMBER</t>
   </si>
   <si>
+    <t xml:space="preserve">Section</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID No</t>
+  </si>
+  <si>
     <t xml:space="preserve">Abajero</t>
   </si>
   <si>
@@ -61,6 +67,9 @@
     <t xml:space="preserve">-</t>
   </si>
   <si>
+    <t xml:space="preserve">18-0036</t>
+  </si>
+  <si>
     <t xml:space="preserve">0007170685</t>
   </si>
   <si>
@@ -82,6 +91,9 @@
     <t xml:space="preserve">09260622531</t>
   </si>
   <si>
+    <t xml:space="preserve">16-0137</t>
+  </si>
+  <si>
     <t xml:space="preserve">0007170668</t>
   </si>
   <si>
@@ -103,6 +115,9 @@
     <t xml:space="preserve">09065245967</t>
   </si>
   <si>
+    <t xml:space="preserve">17-0011</t>
+  </si>
+  <si>
     <t xml:space="preserve">0007170663</t>
   </si>
   <si>
@@ -124,6 +139,9 @@
     <t xml:space="preserve">09298117192</t>
   </si>
   <si>
+    <t xml:space="preserve">17-0008</t>
+  </si>
+  <si>
     <t xml:space="preserve">0007170618</t>
   </si>
   <si>
@@ -145,6 +163,9 @@
     <t xml:space="preserve">09294341620</t>
   </si>
   <si>
+    <t xml:space="preserve">17-0044</t>
+  </si>
+  <si>
     <t xml:space="preserve">0007170601</t>
   </si>
   <si>
@@ -154,6 +175,9 @@
     <t xml:space="preserve">Limuel Andalis </t>
   </si>
   <si>
+    <t xml:space="preserve">17-0045</t>
+  </si>
+  <si>
     <t xml:space="preserve">0007103719</t>
   </si>
   <si>
@@ -175,6 +199,9 @@
     <t xml:space="preserve">09161478519</t>
   </si>
   <si>
+    <t xml:space="preserve">16-0003</t>
+  </si>
+  <si>
     <t xml:space="preserve">Barayoga</t>
   </si>
   <si>
@@ -193,6 +220,9 @@
     <t xml:space="preserve">09079400449</t>
   </si>
   <si>
+    <t xml:space="preserve">16-0031</t>
+  </si>
+  <si>
     <t xml:space="preserve">0007103716</t>
   </si>
   <si>
@@ -214,6 +244,9 @@
     <t xml:space="preserve">09989765743</t>
   </si>
   <si>
+    <t xml:space="preserve">16-0011</t>
+  </si>
+  <si>
     <t xml:space="preserve">0007103697</t>
   </si>
   <si>
@@ -235,6 +268,9 @@
     <t xml:space="preserve">09212423436</t>
   </si>
   <si>
+    <t xml:space="preserve">16-0129</t>
+  </si>
+  <si>
     <t xml:space="preserve">0007103694</t>
   </si>
   <si>
@@ -256,6 +292,9 @@
     <t xml:space="preserve">09090414039</t>
   </si>
   <si>
+    <t xml:space="preserve">16-0030</t>
+  </si>
+  <si>
     <t xml:space="preserve">0007103675</t>
   </si>
   <si>
@@ -274,6 +313,9 @@
     <t xml:space="preserve">09480086686</t>
   </si>
   <si>
+    <t xml:space="preserve">16-0013</t>
+  </si>
+  <si>
     <t xml:space="preserve">0007103514</t>
   </si>
   <si>
@@ -295,6 +337,9 @@
     <t xml:space="preserve">09053638145</t>
   </si>
   <si>
+    <t xml:space="preserve">16-0008</t>
+  </si>
+  <si>
     <t xml:space="preserve">0007103630</t>
   </si>
   <si>
@@ -316,6 +361,9 @@
     <t xml:space="preserve">09099153547</t>
   </si>
   <si>
+    <t xml:space="preserve">16-0159</t>
+  </si>
+  <si>
     <t xml:space="preserve">0007103650</t>
   </si>
   <si>
@@ -337,6 +385,9 @@
     <t xml:space="preserve">09208186541</t>
   </si>
   <si>
+    <t xml:space="preserve">16-0109</t>
+  </si>
+  <si>
     <t xml:space="preserve">Gonzales</t>
   </si>
   <si>
@@ -355,6 +406,9 @@
     <t xml:space="preserve">09977834024</t>
   </si>
   <si>
+    <t xml:space="preserve">16-0014</t>
+  </si>
+  <si>
     <t xml:space="preserve">0007103653</t>
   </si>
   <si>
@@ -376,6 +430,9 @@
     <t xml:space="preserve">09675674735</t>
   </si>
   <si>
+    <t xml:space="preserve">16-0054</t>
+  </si>
+  <si>
     <t xml:space="preserve">0007103672</t>
   </si>
   <si>
@@ -397,6 +454,9 @@
     <t xml:space="preserve">09471871266</t>
   </si>
   <si>
+    <t xml:space="preserve">16-0194</t>
+  </si>
+  <si>
     <t xml:space="preserve">0007097790</t>
   </si>
   <si>
@@ -415,6 +475,9 @@
     <t xml:space="preserve">09495842975</t>
   </si>
   <si>
+    <t xml:space="preserve">17-0018</t>
+  </si>
+  <si>
     <t xml:space="preserve">0007097793</t>
   </si>
   <si>
@@ -433,6 +496,9 @@
     <t xml:space="preserve">09462084094</t>
   </si>
   <si>
+    <t xml:space="preserve">17-0010</t>
+  </si>
+  <si>
     <t xml:space="preserve">0007097812</t>
   </si>
   <si>
@@ -454,6 +520,9 @@
     <t xml:space="preserve">09397595203</t>
   </si>
   <si>
+    <t xml:space="preserve">16-0028</t>
+  </si>
+  <si>
     <t xml:space="preserve">0007097815</t>
   </si>
   <si>
@@ -475,6 +544,9 @@
     <t xml:space="preserve">09481527042</t>
   </si>
   <si>
+    <t xml:space="preserve">18-0224</t>
+  </si>
+  <si>
     <t xml:space="preserve">0007097834</t>
   </si>
   <si>
@@ -496,6 +568,9 @@
     <t xml:space="preserve">09951383831</t>
   </si>
   <si>
+    <t xml:space="preserve">16-0052</t>
+  </si>
+  <si>
     <t xml:space="preserve">0007097881</t>
   </si>
   <si>
@@ -514,6 +589,9 @@
     <t xml:space="preserve">09287866690</t>
   </si>
   <si>
+    <t xml:space="preserve">16-0025</t>
+  </si>
+  <si>
     <t xml:space="preserve">0007097878</t>
   </si>
   <si>
@@ -535,6 +613,9 @@
     <t xml:space="preserve">09487630195</t>
   </si>
   <si>
+    <t xml:space="preserve">16-0183</t>
+  </si>
+  <si>
     <t xml:space="preserve">0007097859</t>
   </si>
   <si>
@@ -556,6 +637,9 @@
     <t xml:space="preserve">09468544328</t>
   </si>
   <si>
+    <t xml:space="preserve">17-0049</t>
+  </si>
+  <si>
     <t xml:space="preserve">0007097856</t>
   </si>
   <si>
@@ -574,6 +658,9 @@
     <t xml:space="preserve">09481489950</t>
   </si>
   <si>
+    <t xml:space="preserve">16-0138</t>
+  </si>
+  <si>
     <t xml:space="preserve">0007097837</t>
   </si>
   <si>
@@ -595,6 +682,9 @@
     <t xml:space="preserve">09098595715</t>
   </si>
   <si>
+    <t xml:space="preserve">17-0054</t>
+  </si>
+  <si>
     <t xml:space="preserve">0007176516</t>
   </si>
   <si>
@@ -616,6 +706,9 @@
     <t xml:space="preserve">09096271466</t>
   </si>
   <si>
+    <t xml:space="preserve">17-0079</t>
+  </si>
+  <si>
     <t xml:space="preserve">0007176523</t>
   </si>
   <si>
@@ -637,6 +730,9 @@
     <t xml:space="preserve">09074244918</t>
   </si>
   <si>
+    <t xml:space="preserve">16-0204</t>
+  </si>
+  <si>
     <t xml:space="preserve">0007176538</t>
   </si>
   <si>
@@ -658,6 +754,9 @@
     <t xml:space="preserve">09121204214</t>
   </si>
   <si>
+    <t xml:space="preserve">16-0168</t>
+  </si>
+  <si>
     <t xml:space="preserve">0007176545</t>
   </si>
   <si>
@@ -677,6 +776,9 @@
   </si>
   <si>
     <t xml:space="preserve">09103727895</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16-0154</t>
   </si>
 </sst>
 </file>
@@ -912,21 +1014,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E15" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3:H33"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2:I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="44.8367346938776"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="35.0969387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.1836734693878"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="44.2755102040816"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.6938775510204"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.780612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -951,826 +1054,928 @@
       <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>35</v>
-      </c>
       <c r="C7" s="5" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="5" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>89</v>
+        <v>103</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>90</v>
+        <v>104</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
-        <v>91</v>
+        <v>106</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>93</v>
+        <v>108</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>96</v>
+        <v>111</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>97</v>
+        <v>112</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
-        <v>98</v>
+        <v>114</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>101</v>
+        <v>117</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>102</v>
+        <v>118</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="10" t="s">
-        <v>105</v>
+        <v>122</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>106</v>
+        <v>123</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>107</v>
+        <v>124</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>108</v>
+        <v>125</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>109</v>
+        <v>126</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>110</v>
+        <v>127</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="I17" s="10" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
-        <v>111</v>
+        <v>129</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>112</v>
+        <v>130</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>113</v>
+        <v>131</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>114</v>
+        <v>132</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>115</v>
+        <v>133</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>116</v>
+        <v>134</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>117</v>
+        <v>135</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
-        <v>118</v>
+        <v>137</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>119</v>
+        <v>138</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>120</v>
+        <v>139</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>121</v>
+        <v>140</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>122</v>
+        <v>141</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>123</v>
+        <v>142</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>124</v>
+        <v>143</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
-        <v>125</v>
+        <v>145</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>126</v>
+        <v>146</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>127</v>
+        <v>147</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>128</v>
+        <v>148</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>129</v>
+        <v>149</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
-        <v>131</v>
+        <v>152</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>132</v>
+        <v>153</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>133</v>
+        <v>154</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>134</v>
+        <v>155</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>135</v>
+        <v>156</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>136</v>
+        <v>157</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
-        <v>137</v>
+        <v>159</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>138</v>
+        <v>160</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>139</v>
+        <v>161</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>140</v>
+        <v>162</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>141</v>
+        <v>163</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>142</v>
+        <v>164</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>143</v>
+        <v>165</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
-        <v>144</v>
+        <v>167</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>145</v>
+        <v>168</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>146</v>
+        <v>169</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>147</v>
+        <v>170</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>148</v>
+        <v>171</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>149</v>
+        <v>172</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>150</v>
+        <v>173</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
-        <v>151</v>
+        <v>175</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>152</v>
+        <v>176</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>153</v>
+        <v>177</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>154</v>
+        <v>178</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>155</v>
+        <v>179</v>
       </c>
       <c r="F24" s="13" t="s">
-        <v>156</v>
+        <v>180</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>157</v>
+        <v>181</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="s">
-        <v>158</v>
+        <v>183</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>159</v>
+        <v>184</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>160</v>
+        <v>185</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>161</v>
+        <v>186</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="F25" s="14" t="s">
-        <v>162</v>
+        <v>187</v>
       </c>
       <c r="G25" s="11" t="s">
-        <v>163</v>
+        <v>188</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="I25" s="10" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="s">
-        <v>164</v>
+        <v>190</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>165</v>
+        <v>191</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>166</v>
+        <v>192</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>167</v>
+        <v>193</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>168</v>
+        <v>194</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>169</v>
+        <v>195</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="s">
-        <v>171</v>
+        <v>198</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>172</v>
+        <v>199</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>173</v>
+        <v>200</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>174</v>
+        <v>201</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>175</v>
+        <v>202</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>176</v>
+        <v>203</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>177</v>
+        <v>204</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="s">
-        <v>178</v>
+        <v>206</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>179</v>
+        <v>207</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>180</v>
+        <v>208</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>181</v>
+        <v>209</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>182</v>
+        <v>210</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>183</v>
+        <v>211</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="s">
-        <v>184</v>
+        <v>213</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>185</v>
+        <v>214</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>186</v>
+        <v>215</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>187</v>
+        <v>216</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>188</v>
+        <v>217</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>189</v>
+        <v>218</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>190</v>
+        <v>219</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="s">
-        <v>191</v>
+        <v>221</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>192</v>
+        <v>222</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>193</v>
+        <v>223</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>194</v>
+        <v>224</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>195</v>
+        <v>225</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>196</v>
+        <v>226</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>197</v>
+        <v>227</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="I30" s="5" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="s">
-        <v>198</v>
+        <v>229</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>199</v>
+        <v>230</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>200</v>
+        <v>231</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>201</v>
+        <v>232</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>202</v>
+        <v>233</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>203</v>
+        <v>234</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>204</v>
+        <v>235</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="4" t="s">
-        <v>205</v>
+        <v>237</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>206</v>
+        <v>238</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>207</v>
+        <v>239</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>208</v>
+        <v>240</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>209</v>
+        <v>241</v>
       </c>
       <c r="F32" s="14" t="s">
-        <v>210</v>
+        <v>242</v>
       </c>
       <c r="G32" s="11" t="s">
-        <v>211</v>
+        <v>243</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="I32" s="10" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="s">
-        <v>212</v>
+        <v>245</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>213</v>
+        <v>246</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>214</v>
+        <v>247</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>215</v>
+        <v>248</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>216</v>
+        <v>249</v>
       </c>
       <c r="F33" s="13" t="s">
-        <v>217</v>
+        <v>250</v>
       </c>
       <c r="G33" s="9" t="s">
-        <v>218</v>
+        <v>251</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="I33" s="8" t="s">
+        <v>252</v>
       </c>
     </row>
   </sheetData>

</xml_diff>